<commit_message>
prepared for journal submission
</commit_message>
<xml_diff>
--- a/supp_materials/supp_table3.xlsx
+++ b/supp_materials/supp_table3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef359c8f53fcc50a/University of Minnesota/PhD/hirsch_lab/projects/marker-effects_networks/supp_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{F297F6E1-DFCF-DA4E-B25A-A6585DC6C648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CDD0932-1ECC-5C49-B060-8ECC3012B85F}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{F297F6E1-DFCF-DA4E-B25A-A6585DC6C648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95C5CFAA-89C2-8B49-8C63-F040D2F7B383}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
   <si>
     <t>Combination</t>
   </si>
@@ -40,7 +40,7 @@
     <t>Minmax</t>
   </si>
   <si>
-    <t>RR-BLUP</t>
+    <t>Z-score</t>
   </si>
 </sst>
 </file>
@@ -602,12 +602,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -895,7 +891,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -903,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,13 +1042,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D10" s="2">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1060,13 +1056,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D11" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1074,13 +1070,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D12" s="2">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1088,13 +1084,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D13" s="2">
-        <v>0.125</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1102,13 +1098,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D14" s="2">
-        <v>0.15</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1116,13 +1112,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D15" s="2">
-        <v>0.17499999999999999</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1130,13 +1126,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D16" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1144,13 +1140,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D17" s="2">
-        <v>0.25</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1161,275 +1157,23 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="3">
+      <c r="D19" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>